<commit_message>
cambios finales de las plantillas y enlace
</commit_message>
<xml_diff>
--- a/public/excel/template-productos.xlsx
+++ b/public/excel/template-productos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyke\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="345" windowWidth="17520" windowHeight="11775"/>
+    <workbookView xWindow="120" yWindow="350" windowWidth="17520" windowHeight="11780"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="4" r:id="rId1"/>
@@ -136,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,6 +261,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -303,7 +311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,7 +346,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -549,31 +557,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7265625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="17" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" customWidth="1"/>
-    <col min="19" max="19" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="15.7109375" style="1"/>
+    <col min="6" max="6" width="23.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="17" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.26953125" customWidth="1"/>
+    <col min="19" max="19" width="23.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="15.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
@@ -644,7 +652,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>9</v>
       </c>
@@ -709,13 +717,13 @@
         <v>35</v>
       </c>
       <c r="V2" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W2" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>10</v>
       </c>
@@ -780,13 +788,13 @@
         <v>35</v>
       </c>
       <c r="V3" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W3" s="5">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>11</v>
       </c>
@@ -851,13 +859,13 @@
         <v>35</v>
       </c>
       <c r="V4" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="W4" s="5">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>12</v>
       </c>
@@ -922,10 +930,10 @@
         <v>35</v>
       </c>
       <c r="V5" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="W5" s="5">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -940,7 +948,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -952,7 +960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -964,7 +972,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>